<commit_message>
Use v3.17 ALFAM2 w 1000 limit on r2
</commit_message>
<xml_diff>
--- a/sens-tab/inputs/inputs.xlsx
+++ b/sens-tab/inputs/inputs.xlsx
@@ -255,6 +255,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -377,13 +378,13 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.83203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.11"/>
@@ -1704,7 +1705,7 @@
       <c r="D28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E28" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="4" t="n">
@@ -1732,7 +1733,7 @@
       <c r="M28" s="4" t="n">
         <v>0.167</v>
       </c>
-      <c r="N28" s="2" t="n">
+      <c r="N28" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O28" s="2" t="n">
@@ -1841,7 +1842,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="atEnd" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;K000000&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"&amp;K000000Page &amp;P</oddFooter>

</xml_diff>